<commit_message>
Cambios excel estudiante 1
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 4-5 - Estudiante 1.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 4-5 - Estudiante 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Segundo Semestre\EDA\Retos\Reto 1\Reto1-G03\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AEBD3D18-DBCC-494B-9E1B-9D93992A8FC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D782FB-3B1F-489E-95AF-235AE866092A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="1" activeTab="6" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -155,61 +155,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -498,6 +451,56 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -570,7 +573,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -637,7 +640,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -724,7 +727,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -775,34 +778,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>562.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>2343.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>8875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>37125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>146906.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>620171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -892,7 +883,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -943,34 +934,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2609.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10656.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>43203.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>182875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>756250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,7 +1038,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1103,7 +1082,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1154,34 +1133,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>156.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>390.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>968.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2109.375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12218.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>30062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,7 +1254,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1329,34 +1305,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>156.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>1171.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>2515.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>12234.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,7 +1426,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1504,34 +1477,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>109.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>234.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>484.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>1093.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>2296.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>5062.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>10843.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1631,7 +1601,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1669,7 +1639,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1753,7 +1723,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1791,7 +1761,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1833,7 +1803,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1870,7 +1840,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1879,7 +1849,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1946,7 +1916,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2043,7 +2013,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2094,34 +2064,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>38234.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>326781.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2668125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2210,7 +2159,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2261,34 +2210,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>37546.864999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>274531</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2288343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2377,7 +2305,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2428,34 +2356,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2171.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>8906.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>39078.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>204359.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1002468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,7 +2465,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2603,34 +2516,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>1468.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>7281.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>30750</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>135703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>541468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2727,7 +2625,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2778,34 +2676,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>218.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>921.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>3718.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>12484.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>58468.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>224625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2905,7 +2791,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2943,7 +2829,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -3027,7 +2913,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3065,7 +2951,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -3107,7 +2993,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3144,7 +3030,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3153,7 +3039,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3220,7 +3106,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3307,7 +3193,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3358,34 +3244,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>562.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>2343.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>8875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>37125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>146906.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>620171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3474,7 +3348,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3525,34 +3399,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>38234.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>326781.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2668125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3652,7 +3505,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3690,7 +3543,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3769,7 +3622,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3807,7 +3660,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3849,7 +3702,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3886,7 +3739,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3895,7 +3748,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3957,7 +3810,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4044,7 +3897,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4095,34 +3948,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2609.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10656.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>43203.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>182875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>756250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4211,7 +4052,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4262,34 +4103,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>37546.864999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>274531</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2288343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4389,7 +4209,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4427,7 +4247,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4506,7 +4326,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4544,7 +4364,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4586,7 +4406,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4623,7 +4443,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -4632,7 +4452,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4694,7 +4514,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4781,7 +4601,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4832,34 +4652,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>156.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>390.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>968.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2109.375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12218.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>30062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4948,7 +4765,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4999,34 +4816,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2171.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>8906.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>39078.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>204359.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1002468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5126,7 +4928,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5164,7 +4966,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5243,7 +5045,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5281,7 +5083,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -5323,7 +5125,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5360,7 +5162,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -5369,7 +5171,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5439,7 +5241,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5526,7 +5328,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5577,34 +5379,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>156.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>1171.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>2515.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>12234.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5693,7 +5492,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5744,34 +5543,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>1468.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>7281.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>30750</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>135703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>541468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5871,7 +5655,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5909,7 +5693,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5988,7 +5772,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6026,7 +5810,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -6068,7 +5852,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6105,7 +5889,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -6114,7 +5898,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6184,7 +5968,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6272,7 +6056,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6323,34 +6107,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>109.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>234.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>484.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>1093.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>2296.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>5062.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>10843.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6440,7 +6221,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6491,34 +6272,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>218.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>921.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>3718.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>12484.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>58468.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>224625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6618,7 +6387,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6656,7 +6425,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -6735,7 +6504,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6773,7 +6542,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -6815,7 +6584,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6852,7 +6621,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -10748,7 +10517,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10803,7 +10572,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10825,7 +10594,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661400" cy="6286500"/>
+    <xdr:ext cx="8696325" cy="6305550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10858,7 +10627,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10891,7 +10660,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10924,7 +10693,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10957,7 +10726,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10990,7 +10759,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11023,7 +10792,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8694615" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11060,21 +10829,21 @@
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Quick Sort [ms]" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{21628D13-D0BA-41D1-8E51-AB02437FBDE5}" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
@@ -11083,7 +10852,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -11382,19 +11151,19 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22.1171875" customWidth="1"/>
+    <col min="5" max="6" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -11414,224 +11183,185 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4">
-        <v>15.7</v>
+      <c r="B2" s="6">
+        <v>562.5</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
+      <c r="C2" s="6">
+        <v>625</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="D2" s="6">
+        <v>46.875</v>
       </c>
       <c r="E2" s="5">
-        <v>20</v>
+        <v>15.625</v>
       </c>
       <c r="F2" s="5">
-        <v>60</v>
+        <v>31.25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4">
-        <v>30</v>
+      <c r="B3" s="6">
+        <v>2343.75</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
+      <c r="C3" s="6">
+        <v>2609.375</v>
       </c>
-      <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+      <c r="D3" s="6">
+        <v>78.125</v>
       </c>
       <c r="E3" s="5">
-        <v>40</v>
+        <v>62.5</v>
       </c>
       <c r="F3" s="5">
-        <v>90</v>
+        <v>62.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="4">
-        <v>45</v>
+      <c r="B4" s="6">
+        <v>8875</v>
       </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+      <c r="C4" s="6">
+        <v>10656.25</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+      <c r="D4" s="6">
+        <v>156.25</v>
       </c>
       <c r="E4" s="5">
-        <v>60</v>
+        <v>156.25</v>
       </c>
       <c r="F4" s="5">
-        <v>120</v>
+        <v>109.375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="4">
-        <v>60</v>
+      <c r="B5" s="6">
+        <v>37125</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+      <c r="C5" s="6">
+        <v>43203.125</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="D5" s="6">
+        <v>390.625</v>
       </c>
       <c r="E5" s="5">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="F5" s="5">
-        <v>150</v>
+        <v>234.375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="4">
-        <v>75</v>
+      <c r="B6" s="6">
+        <v>146906.5</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+      <c r="C6" s="6">
+        <v>182875</v>
       </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+      <c r="D6" s="6">
+        <v>968.75</v>
       </c>
       <c r="E6" s="5">
-        <v>100</v>
+        <v>531.25</v>
       </c>
       <c r="F6" s="5">
-        <v>180</v>
+        <v>484.375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="4">
-        <v>90</v>
+      <c r="B7" s="6">
+        <v>620171</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+      <c r="C7" s="6">
+        <v>756250</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+      <c r="D7" s="6">
+        <v>2109.375</v>
       </c>
       <c r="E7" s="5">
-        <v>120</v>
+        <v>1171.875</v>
       </c>
       <c r="F7" s="5">
-        <v>210</v>
+        <v>1093.75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>105</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
+        <v>5125</v>
       </c>
       <c r="E8" s="5">
-        <v>140</v>
+        <v>2515.625</v>
       </c>
       <c r="F8" s="5">
-        <v>240</v>
+        <v>2296.875</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>120</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <v>12218.75</v>
       </c>
       <c r="E9" s="5">
-        <v>160</v>
+        <v>5000</v>
       </c>
       <c r="F9" s="5">
-        <v>270</v>
+        <v>5062.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>135</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <v>30062</v>
       </c>
       <c r="E10" s="5">
-        <v>180</v>
+        <v>12234.375</v>
       </c>
       <c r="F10" s="5">
-        <v>300</v>
+        <v>10843.75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>150</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="E11" s="5">
-        <v>200</v>
-      </c>
-      <c r="F11" s="5">
-        <v>330</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -11651,222 +11381,149 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4">
-        <v>50</v>
+      <c r="B15" s="6">
+        <v>38234.375</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
+      <c r="C15" s="6">
+        <v>37546.864999999998</v>
       </c>
-      <c r="D15" s="4">
-        <v>35</v>
+      <c r="D15" s="6">
+        <v>2171.875</v>
       </c>
       <c r="E15" s="5">
-        <v>30</v>
+        <v>1468.75</v>
       </c>
       <c r="F15" s="5">
-        <v>70</v>
+        <v>218.75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4">
-        <v>60</v>
+      <c r="B16" s="6">
+        <v>326781.25</v>
       </c>
-      <c r="C16" s="4">
-        <v>4</v>
+      <c r="C16" s="6">
+        <v>274531</v>
       </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+      <c r="D16" s="6">
+        <v>8906.25</v>
       </c>
       <c r="E16" s="5">
-        <v>60</v>
+        <v>7281.25</v>
       </c>
       <c r="F16" s="5">
-        <v>90</v>
+        <v>921.875</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="4">
-        <v>70</v>
+      <c r="B17" s="6">
+        <v>2668125</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+      <c r="C17" s="6">
+        <v>2288343</v>
       </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+      <c r="D17" s="6">
+        <v>39078.125</v>
       </c>
       <c r="E17" s="5">
-        <v>90</v>
+        <v>30750</v>
       </c>
       <c r="F17" s="5">
-        <v>110</v>
+        <v>3718.75</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
+        <v>204359.375</v>
       </c>
       <c r="E18" s="5">
-        <v>120</v>
+        <v>135703</v>
       </c>
       <c r="F18" s="5">
-        <v>130</v>
+        <v>12484.375</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>1002468</v>
       </c>
       <c r="E19" s="5">
-        <v>150</v>
+        <v>541468</v>
       </c>
       <c r="F19" s="5">
-        <v>150</v>
+        <v>58468.75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
-      <c r="E20" s="5">
-        <v>180</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5">
-        <v>170</v>
+        <v>224625</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
-      <c r="E21" s="5">
-        <v>210</v>
-      </c>
-      <c r="F21" s="5">
-        <v>190</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
-      <c r="E22" s="5">
-        <v>240</v>
-      </c>
-      <c r="F22" s="5">
-        <v>210</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
-      <c r="E23" s="5">
-        <v>270</v>
-      </c>
-      <c r="F23" s="5">
-        <v>230</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
-      <c r="E24" s="5">
-        <v>300</v>
-      </c>
-      <c r="F24" s="5">
-        <v>250</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11878,6 +11535,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c10596efcc8303131ba000bf7988b65d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88645b4f568d2e9f6d2a1da3b5a5f323" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -12088,34 +11760,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EE155A0-3C6B-4FBA-920A-A0416B6AA614}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -12130,4 +11775,31 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EE155A0-3C6B-4FBA-920A-A0416B6AA614}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>